<commit_message>
[Feature] Convert to real data in dashboard and FIX 404 Error in StationDetail
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niqa Nabila\Documents\Kuliah\Magang\BMKG\Tugas BMKG\Project-besar\Stasiun quality control\Station-Quality-Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E3C3F9-1662-494A-ABC7-E74BF9609E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C381A87A-1EC6-4C41-B4DD-637FED3F4065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4394,8 +4394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C22"/>
+    <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
+      <selection activeCell="J401" sqref="J401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
[Feature] Add feature to Detail page and fix triangle map in dashboard
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niqa Nabila\Documents\Kuliah\Magang\BMKG\Tugas BMKG\Project-besar\Stasiun quality control\Station-Quality-Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C381A87A-1EC6-4C41-B4DD-637FED3F4065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DC7FF8-5BD6-496E-ADBF-7A359097F2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4394,8 +4394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
-      <selection activeCell="J401" sqref="J401"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="J103" sqref="J103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>